<commit_message>
The thrust calculations have been done, total thrust is added to the excel file in Testflightdata/20200305_V3_metric
</commit_message>
<xml_diff>
--- a/Testflightdata/20200305_V3_metric.xlsx
+++ b/Testflightdata/20200305_V3_metric.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitch\Documents\TU Delft\BSc-3\AE3212-II Simulation, Verification &amp; Validation\Aerodynamics\31\B31\Testflightdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/088ac5db3e9756e7/Documents/MATLAB/31/B31/Testflightdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9CE49C-422C-4B40-AFF9-19CAFA55059E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="247" documentId="13_ncr:1_{6C9CE49C-422C-4B40-AFF9-19CAFA55059E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{85A24241-D93A-4EE9-B448-5B215C5551D4}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{D344435E-CCBC-4168-9073-2AFFB31A2551}"/>
+    <workbookView xWindow="16480" yWindow="1440" windowWidth="21080" windowHeight="15450" xr2:uid="{D344435E-CCBC-4168-9073-2AFFB31A2551}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="69">
   <si>
     <t>Post-Flight Data Sheet AE3202 - Metric</t>
   </si>
@@ -210,15 +210,50 @@
   </si>
   <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>Mach</t>
+  </si>
+  <si>
+    <t>Needed for Thrust calculations</t>
+  </si>
+  <si>
+    <t>[-]</t>
+  </si>
+  <si>
+    <t>[kg/s]</t>
+  </si>
+  <si>
+    <t>T_ISA</t>
+  </si>
+  <si>
+    <t>DeltaT ISA</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>K/deg C</t>
+  </si>
+  <si>
+    <t>T_left</t>
+  </si>
+  <si>
+    <t>T_right</t>
+  </si>
+  <si>
+    <t>Thrust</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -237,12 +272,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -257,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -266,6 +307,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -287,8 +333,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Imperial Units"/>
-      <sheetName val="Metric Units"/>
+      <sheetName val="Sheet1"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
@@ -894,7 +939,6 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1197,23 +1241,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34902A54-5175-498F-89F5-74E384953902}">
-  <dimension ref="A1:M84"/>
+  <dimension ref="A1:AE84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G88" sqref="G88"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AC74" sqref="AC74:AE74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="10.15625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.08984375" customWidth="1"/>
+    <col min="19" max="19" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13" customWidth="1"/>
+    <col min="21" max="21" width="10.54296875" customWidth="1"/>
+    <col min="23" max="23" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="8.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1224,7 +1275,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1235,12 +1286,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
         <v>16</v>
       </c>
@@ -1248,134 +1299,134 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="str">
-        <f>'[1]Imperial Units'!$D8</f>
+        <f>[1]Sheet1!$D8</f>
         <v>Chipke</v>
       </c>
       <c r="G8">
-        <f>'[1]Imperial Units'!$H8</f>
+        <f>[1]Sheet1!$H8</f>
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="C9" t="str">
-        <f>'[1]Imperial Units'!$D9</f>
+        <f>[1]Sheet1!$D9</f>
         <v>Hans</v>
       </c>
       <c r="G9">
-        <f>'[1]Imperial Units'!$H9</f>
+        <f>[1]Sheet1!$H9</f>
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="str">
-        <f>'[1]Imperial Units'!$D10</f>
+        <f>[1]Sheet1!$D10</f>
         <v>Marta</v>
       </c>
       <c r="G10">
-        <f>'[1]Imperial Units'!$H10</f>
+        <f>[1]Sheet1!$H10</f>
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="str">
-        <f>'[1]Imperial Units'!$D11</f>
+        <f>[1]Sheet1!$D11</f>
         <v>Jari</v>
       </c>
       <c r="G11">
-        <f>'[1]Imperial Units'!$H11</f>
+        <f>[1]Sheet1!$H11</f>
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="C12" t="str">
-        <f>'[1]Imperial Units'!$D12</f>
+        <f>[1]Sheet1!$D12</f>
         <v>Martin</v>
       </c>
       <c r="G12">
-        <f>'[1]Imperial Units'!$H12</f>
+        <f>[1]Sheet1!$H12</f>
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="C13" t="str">
-        <f>'[1]Imperial Units'!$D13</f>
+        <f>[1]Sheet1!$D13</f>
         <v>Wessel</v>
       </c>
       <c r="G13">
-        <f>'[1]Imperial Units'!$H13</f>
+        <f>[1]Sheet1!$H13</f>
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="C14" t="str">
-        <f>'[1]Imperial Units'!$D14</f>
+        <f>[1]Sheet1!$D14</f>
         <v>Simon</v>
       </c>
       <c r="G14">
-        <f>'[1]Imperial Units'!$H14</f>
+        <f>[1]Sheet1!$H14</f>
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="C15" t="str">
-        <f>'[1]Imperial Units'!$D15</f>
+        <f>[1]Sheet1!$D15</f>
         <v>Niek</v>
       </c>
       <c r="G15">
-        <f>'[1]Imperial Units'!$H15</f>
+        <f>[1]Sheet1!$H15</f>
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="C16" t="str">
-        <f>'[1]Imperial Units'!$D16</f>
+        <f>[1]Sheet1!$D16</f>
         <v>Julian</v>
       </c>
       <c r="G16">
-        <f>'[1]Imperial Units'!$H16</f>
+        <f>[1]Sheet1!$H16</f>
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -1383,7 +1434,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="W24" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -1393,7 +1449,7 @@
       <c r="C25" t="s">
         <v>20</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="9" t="s">
         <v>21</v>
       </c>
       <c r="E25" t="s">
@@ -1414,8 +1470,35 @@
       <c r="J25" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="T25" t="s">
+        <v>62</v>
+      </c>
+      <c r="W25" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="X25" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y25" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z25" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA25" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC25" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD25" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE25" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>28</v>
       </c>
@@ -1443,213 +1526,418 @@
       <c r="J26" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="T26" t="s">
+        <v>64</v>
+      </c>
+      <c r="W26" t="s">
+        <v>30</v>
+      </c>
+      <c r="X26" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD26" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>1</v>
       </c>
       <c r="B28" s="3">
-        <f>'[1]Imperial Units'!B28</f>
+        <f>[1]Sheet1!B28</f>
         <v>0.65208333333333335</v>
       </c>
       <c r="C28" s="3">
         <f>B28-$B$28</f>
         <v>0</v>
       </c>
-      <c r="D28" s="4">
-        <f>'[1]Imperial Units'!D28*0.3048</f>
+      <c r="D28" s="11">
+        <f>[1]Sheet1!D28*0.3048</f>
         <v>1530.096</v>
       </c>
-      <c r="E28" s="4">
-        <f>'[1]Imperial Units'!E28/0.514444</f>
-        <v>482.07385060375861</v>
+      <c r="E28" s="11">
+        <f>[1]Sheet1!E28*0.514444</f>
+        <v>127.58211200000001</v>
       </c>
       <c r="F28" s="4">
-        <f>'[1]Imperial Units'!F28</f>
+        <f>[1]Sheet1!F28</f>
         <v>1.8</v>
       </c>
       <c r="G28" s="4">
-        <f>'[1]Imperial Units'!G28*0.45359237</f>
+        <f>[1]Sheet1!G28*0.45359237</f>
         <v>340.1942775</v>
       </c>
       <c r="H28" s="4">
-        <f>'[1]Imperial Units'!H28*0.45359237</f>
+        <f>[1]Sheet1!H28*0.45359237</f>
         <v>364.23467311000002</v>
       </c>
       <c r="I28" s="4">
-        <f>'[1]Imperial Units'!I28*0.45359237</f>
+        <f>[1]Sheet1!I28*0.45359237</f>
         <v>134.71693389000001</v>
       </c>
       <c r="J28" s="4">
-        <f>'[1]Imperial Units'!J28</f>
+        <f>[1]Sheet1!J28</f>
         <v>10.199999999999999</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="L28">
+        <v>0.28152897243643699</v>
+      </c>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+      <c r="T28">
+        <f>(273.15+15) + 0.0065*D28</f>
+        <v>298.09562399999999</v>
+      </c>
+      <c r="W28" s="12">
+        <f>D28</f>
+        <v>1530.096</v>
+      </c>
+      <c r="X28" s="12">
+        <v>0.74259570370114603</v>
+      </c>
+      <c r="Y28" s="12">
+        <f>(J28+273.15)-T28</f>
+        <v>-14.745624000000021</v>
+      </c>
+      <c r="Z28" s="12">
+        <f>G28/3600</f>
+        <v>9.4498410416666664E-2</v>
+      </c>
+      <c r="AA28" s="12">
+        <f>H28/3600</f>
+        <v>0.10117629808611112</v>
+      </c>
+      <c r="AC28">
+        <v>2284.7600000000002</v>
+      </c>
+      <c r="AD28">
+        <v>2585.11</v>
+      </c>
+      <c r="AE28">
+        <f>AC28+AD28</f>
+        <v>4869.8700000000008</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2</v>
       </c>
       <c r="B29" s="3">
-        <f>'[1]Imperial Units'!B29</f>
+        <f>[1]Sheet1!B29</f>
         <v>0.72152777777777777</v>
       </c>
       <c r="C29" s="3">
         <f t="shared" ref="C29:C33" si="0">B29-$B$28</f>
         <v>6.944444444444442E-2</v>
       </c>
-      <c r="D29" s="4">
-        <f>'[1]Imperial Units'!D29*0.3048</f>
+      <c r="D29" s="11">
+        <f>[1]Sheet1!D29*0.3048</f>
         <v>1530.096</v>
       </c>
-      <c r="E29" s="4">
-        <f>'[1]Imperial Units'!E29/0.514444</f>
-        <v>429.59000396544616</v>
+      <c r="E29" s="11">
+        <f>[1]Sheet1!E29*0.514444</f>
+        <v>113.69212400000001</v>
       </c>
       <c r="F29" s="4">
-        <f>'[1]Imperial Units'!F29</f>
+        <f>[1]Sheet1!F29</f>
         <v>2.5</v>
       </c>
       <c r="G29" s="4">
-        <f>'[1]Imperial Units'!G29*0.45359237</f>
+        <f>[1]Sheet1!G29*0.45359237</f>
         <v>288.48474732</v>
       </c>
       <c r="H29" s="4">
-        <f>'[1]Imperial Units'!H29*0.45359237</f>
+        <f>[1]Sheet1!H29*0.45359237</f>
         <v>310.71077345000003</v>
       </c>
       <c r="I29" s="4">
-        <f>'[1]Imperial Units'!I29*0.45359237</f>
+        <f>[1]Sheet1!I29*0.45359237</f>
         <v>151.49985158000001</v>
       </c>
       <c r="J29" s="4">
-        <f>'[1]Imperial Units'!J29</f>
+        <f>[1]Sheet1!J29</f>
         <v>8.5</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29">
+        <f>(273.15+15) + 0.0065*D29</f>
+        <v>298.09562399999999</v>
+      </c>
+      <c r="W29" s="12">
+        <f>D29</f>
+        <v>1530.096</v>
+      </c>
+      <c r="X29" s="12">
+        <v>0.70125474911411401</v>
+      </c>
+      <c r="Y29" s="12">
+        <f>(J29+273.15)-T29</f>
+        <v>-16.445624000000009</v>
+      </c>
+      <c r="Z29" s="12">
+        <f>G29/3600</f>
+        <v>8.0134652033333337E-2</v>
+      </c>
+      <c r="AA29" s="12">
+        <f>H29/3600</f>
+        <v>8.6308548180555569E-2</v>
+      </c>
+      <c r="AC29">
+        <v>1785.52</v>
+      </c>
+      <c r="AD29">
+        <v>2056.96</v>
+      </c>
+      <c r="AE29">
+        <f t="shared" ref="AE29:AE33" si="1">AC29+AD29</f>
+        <v>3842.48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>3</v>
       </c>
       <c r="B30" s="3">
-        <f>'[1]Imperial Units'!B30</f>
+        <f>[1]Sheet1!B30</f>
         <v>0.80555555555555547</v>
       </c>
       <c r="C30" s="3">
         <f t="shared" si="0"/>
         <v>0.15347222222222212</v>
       </c>
-      <c r="D30" s="4">
-        <f>'[1]Imperial Units'!D30*0.3048</f>
+      <c r="D30" s="11">
+        <f>[1]Sheet1!D30*0.3048</f>
         <v>1530.096</v>
       </c>
-      <c r="E30" s="4">
-        <f>'[1]Imperial Units'!E30/0.514444</f>
-        <v>365.44308029639768</v>
+      <c r="E30" s="11">
+        <f>[1]Sheet1!E30*0.514444</f>
+        <v>96.715472000000005</v>
       </c>
       <c r="F30" s="4">
-        <f>'[1]Imperial Units'!F30</f>
+        <f>[1]Sheet1!F30</f>
         <v>3.9</v>
       </c>
       <c r="G30" s="4">
-        <f>'[1]Imperial Units'!G30*0.45359237</f>
+        <f>[1]Sheet1!G30*0.45359237</f>
         <v>244.03269506000001</v>
       </c>
       <c r="H30" s="4">
-        <f>'[1]Imperial Units'!H30*0.45359237</f>
+        <f>[1]Sheet1!H30*0.45359237</f>
         <v>263.99075934000001</v>
       </c>
       <c r="I30" s="4">
-        <f>'[1]Imperial Units'!I30*0.45359237</f>
+        <f>[1]Sheet1!I30*0.45359237</f>
         <v>164.20043794</v>
       </c>
       <c r="J30" s="4">
-        <f>'[1]Imperial Units'!J30</f>
+        <f>[1]Sheet1!J30</f>
         <v>6.8</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+      <c r="T30">
+        <f>(273.15+15) + 0.0065*D30</f>
+        <v>298.09562399999999</v>
+      </c>
+      <c r="W30" s="12">
+        <f>D30</f>
+        <v>1530.096</v>
+      </c>
+      <c r="X30" s="12">
+        <v>0.65432077180474402</v>
+      </c>
+      <c r="Y30" s="12">
+        <f>(J30+273.15)-T30</f>
+        <v>-18.145623999999998</v>
+      </c>
+      <c r="Z30" s="12">
+        <f>G30/3600</f>
+        <v>6.7786859738888885E-2</v>
+      </c>
+      <c r="AA30" s="12">
+        <f>H30/3600</f>
+        <v>7.3330766483333337E-2</v>
+      </c>
+      <c r="AC30">
+        <v>1375.8</v>
+      </c>
+      <c r="AD30">
+        <v>1618.5</v>
+      </c>
+      <c r="AE30">
+        <f t="shared" si="1"/>
+        <v>2994.3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>4</v>
       </c>
       <c r="B31" s="3">
-        <f>'[1]Imperial Units'!B31</f>
+        <f>[1]Sheet1!B31</f>
         <v>0.89722222222222225</v>
       </c>
       <c r="C31" s="3">
         <f t="shared" si="0"/>
         <v>0.24513888888888891</v>
       </c>
-      <c r="D31" s="4">
-        <f>'[1]Imperial Units'!D31*0.3048</f>
+      <c r="D31" s="11">
+        <f>[1]Sheet1!D31*0.3048</f>
         <v>1530.096</v>
       </c>
-      <c r="E31" s="4">
-        <f>'[1]Imperial Units'!E31/0.514444</f>
-        <v>311.01538748629588</v>
+      <c r="E31" s="11">
+        <f>[1]Sheet1!E31*0.514444</f>
+        <v>82.311040000000006</v>
       </c>
       <c r="F31" s="4">
-        <f>'[1]Imperial Units'!F31</f>
+        <f>[1]Sheet1!F31</f>
         <v>5.7</v>
       </c>
       <c r="G31" s="4">
-        <f>'[1]Imperial Units'!G31*0.45359237</f>
+        <f>[1]Sheet1!G31*0.45359237</f>
         <v>209.55967494000001</v>
       </c>
       <c r="H31" s="4">
-        <f>'[1]Imperial Units'!H31*0.45359237</f>
+        <f>[1]Sheet1!H31*0.45359237</f>
         <v>225.43540789000002</v>
       </c>
       <c r="I31" s="4">
-        <f>'[1]Imperial Units'!I31*0.45359237</f>
+        <f>[1]Sheet1!I31*0.45359237</f>
         <v>180.98335563000001</v>
       </c>
       <c r="J31" s="4">
-        <f>'[1]Imperial Units'!J31</f>
+        <f>[1]Sheet1!J31</f>
         <v>5.2</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="R31" s="4"/>
+      <c r="S31" s="4"/>
+      <c r="T31">
+        <f>(273.15+15) + 0.0065*D31</f>
+        <v>298.09562399999999</v>
+      </c>
+      <c r="W31" s="12">
+        <f>D31</f>
+        <v>1530.096</v>
+      </c>
+      <c r="X31" s="12">
+        <v>0.61822847102252598</v>
+      </c>
+      <c r="Y31" s="12">
+        <f>(J31+273.15)-T31</f>
+        <v>-19.745624000000021</v>
+      </c>
+      <c r="Z31" s="12">
+        <f>G31/3600</f>
+        <v>5.8211020816666667E-2</v>
+      </c>
+      <c r="AA31" s="12">
+        <f>H31/3600</f>
+        <v>6.2620946636111119E-2</v>
+      </c>
+      <c r="AC31">
+        <v>1046.79</v>
+      </c>
+      <c r="AD31">
+        <v>1239.4100000000001</v>
+      </c>
+      <c r="AE31">
+        <f t="shared" si="1"/>
+        <v>2286.1999999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>5</v>
       </c>
       <c r="B32" s="3">
-        <f>'[1]Imperial Units'!B32</f>
+        <f>[1]Sheet1!B32</f>
         <v>0.95694444444444438</v>
       </c>
       <c r="C32" s="3">
         <f t="shared" si="0"/>
         <v>0.30486111111111103</v>
       </c>
-      <c r="D32" s="4">
-        <f>'[1]Imperial Units'!D32*0.3048</f>
+      <c r="D32" s="11">
+        <f>[1]Sheet1!D32*0.3048</f>
         <v>1527.048</v>
       </c>
-      <c r="E32" s="4">
-        <f>'[1]Imperial Units'!E32/0.514444</f>
-        <v>264.36307936335152</v>
+      <c r="E32" s="11">
+        <f>[1]Sheet1!E32*0.514444</f>
+        <v>69.964383999999995</v>
       </c>
       <c r="F32" s="4">
-        <f>'[1]Imperial Units'!F32</f>
+        <f>[1]Sheet1!F32</f>
         <v>8.1999999999999993</v>
       </c>
       <c r="G32" s="4">
-        <f>'[1]Imperial Units'!G32*0.45359237</f>
+        <f>[1]Sheet1!G32*0.45359237</f>
         <v>197.31268095000001</v>
       </c>
       <c r="H32" s="4">
-        <f>'[1]Imperial Units'!H32*0.45359237</f>
+        <f>[1]Sheet1!H32*0.45359237</f>
         <v>216.81715286000002</v>
       </c>
       <c r="I32" s="4">
-        <f>'[1]Imperial Units'!I32*0.45359237</f>
+        <f>[1]Sheet1!I32*0.45359237</f>
         <v>189.60161066000001</v>
       </c>
       <c r="J32" s="4">
-        <f>'[1]Imperial Units'!J32</f>
+        <f>[1]Sheet1!J32</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="R32" s="4"/>
+      <c r="S32" s="4"/>
+      <c r="T32">
+        <f>(273.15+15) + 0.0065*D32</f>
+        <v>298.07581199999998</v>
+      </c>
+      <c r="W32" s="12">
+        <f>D32</f>
+        <v>1527.048</v>
+      </c>
+      <c r="X32" s="12">
+        <v>0.590072052546873</v>
+      </c>
+      <c r="Y32" s="12">
+        <f>(J32+273.15)-T32</f>
+        <v>-20.925812000000008</v>
+      </c>
+      <c r="Z32" s="12">
+        <f>G32/3600</f>
+        <v>5.4809078041666674E-2</v>
+      </c>
+      <c r="AA32" s="12">
+        <f>H32/3600</f>
+        <v>6.0226986905555564E-2</v>
+      </c>
+      <c r="AC32">
+        <v>962.798</v>
+      </c>
+      <c r="AD32">
+        <v>1204.31</v>
+      </c>
+      <c r="AE32">
+        <f t="shared" si="1"/>
+        <v>2167.1080000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>6</v>
       </c>
@@ -1660,57 +1948,113 @@
         <f t="shared" si="0"/>
         <v>1.3666666666666665</v>
       </c>
-      <c r="D33" s="4">
-        <f>'[1]Imperial Units'!D33*0.3048</f>
+      <c r="D33" s="11">
+        <f>[1]Sheet1!D33*0.3048</f>
         <v>1530.096</v>
       </c>
-      <c r="E33" s="4">
-        <f>'[1]Imperial Units'!E33/0.514444</f>
-        <v>237.14923295830062</v>
+      <c r="E33" s="11">
+        <f>[1]Sheet1!E33*0.514444</f>
+        <v>62.762168000000003</v>
       </c>
       <c r="F33" s="4">
-        <f>'[1]Imperial Units'!F33</f>
+        <f>[1]Sheet1!F33</f>
         <v>10.3</v>
       </c>
       <c r="G33" s="4">
-        <f>'[1]Imperial Units'!G33*0.45359237</f>
+        <f>[1]Sheet1!G33*0.45359237</f>
         <v>195.95190384</v>
       </c>
       <c r="H33" s="4">
-        <f>'[1]Imperial Units'!H33*0.45359237</f>
+        <f>[1]Sheet1!H33*0.45359237</f>
         <v>216.36356049</v>
       </c>
       <c r="I33" s="4">
-        <f>'[1]Imperial Units'!I33*0.45359237</f>
+        <f>[1]Sheet1!I33*0.45359237</f>
         <v>200.03423517000002</v>
       </c>
       <c r="J33" s="4">
-        <f>'[1]Imperial Units'!J33</f>
+        <f>[1]Sheet1!J33</f>
         <v>3.8</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="R33" s="4"/>
+      <c r="S33" s="4"/>
+      <c r="T33">
+        <f>(273.15+15) + 0.0065*D33</f>
+        <v>298.09562399999999</v>
+      </c>
+      <c r="W33" s="12">
+        <f>D33</f>
+        <v>1530.096</v>
+      </c>
+      <c r="X33" s="12">
+        <v>0.57592854095171098</v>
+      </c>
+      <c r="Y33" s="12">
+        <f>(J33+273.15)-T33</f>
+        <v>-21.145623999999998</v>
+      </c>
+      <c r="Z33" s="12">
+        <f>G33/3600</f>
+        <v>5.4431084400000003E-2</v>
+      </c>
+      <c r="AA33" s="12">
+        <f>H33/3600</f>
+        <v>6.0100989025000003E-2</v>
+      </c>
+      <c r="AC33">
+        <v>977.779</v>
+      </c>
+      <c r="AD33">
+        <v>1235.1199999999999</v>
+      </c>
+      <c r="AE33">
+        <f t="shared" si="1"/>
+        <v>2212.8989999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>7</v>
       </c>
       <c r="B34" s="3"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="R34" s="4"/>
+      <c r="S34" s="4"/>
+      <c r="U34" s="4"/>
+    </row>
+    <row r="35" spans="1:31" x14ac:dyDescent="0.35">
       <c r="C35" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="S35" s="4"/>
+      <c r="U35" s="4"/>
+    </row>
+    <row r="36" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="S36" s="4"/>
+      <c r="U36" s="4"/>
+    </row>
+    <row r="37" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="S37" s="4"/>
+      <c r="U37" s="4"/>
+    </row>
+    <row r="38" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="S38" s="4"/>
+      <c r="U38" s="4"/>
+    </row>
+    <row r="39" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="S39" s="4"/>
+      <c r="U39" s="4"/>
+    </row>
+    <row r="40" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="S40" s="4"/>
+      <c r="U40" s="4"/>
+    </row>
+    <row r="41" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>18</v>
       </c>
@@ -1741,8 +2085,10 @@
       <c r="J41" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="S41" s="4"/>
+      <c r="U41" s="4"/>
+    </row>
+    <row r="42" spans="1:31" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>28</v>
       </c>
@@ -1770,13 +2116,19 @@
       <c r="J42" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="S42" s="4"/>
+      <c r="U42" s="4"/>
+    </row>
+    <row r="43" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="S43" s="4"/>
+      <c r="U43" s="4"/>
+    </row>
+    <row r="44" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>1</v>
       </c>
       <c r="B44" s="3">
-        <f>'[1]Imperial Units'!B44</f>
+        <f>[1]Sheet1!B44</f>
         <v>0</v>
       </c>
       <c r="C44" s="3">
@@ -1784,256 +2136,288 @@
         <v>-0.65208333333333335</v>
       </c>
       <c r="D44" s="4">
-        <f>'[1]Imperial Units'!D44*0.3048</f>
+        <f>[1]Sheet1!D44*0.3048</f>
         <v>0</v>
       </c>
       <c r="E44" s="4">
-        <f>'[1]Imperial Units'!E44/0.514444</f>
+        <f>[1]Sheet1!E44/0.514444</f>
         <v>0</v>
       </c>
       <c r="F44" s="4">
-        <f>'[1]Imperial Units'!F44</f>
+        <f>[1]Sheet1!F44</f>
         <v>0</v>
       </c>
       <c r="G44" s="4">
-        <f>'[1]Imperial Units'!G44*0.45359237</f>
+        <f>[1]Sheet1!G44*0.45359237</f>
         <v>0</v>
       </c>
       <c r="H44" s="4">
-        <f>'[1]Imperial Units'!H44*0.45359237</f>
+        <f>[1]Sheet1!H44*0.45359237</f>
         <v>0</v>
       </c>
       <c r="I44" s="4">
-        <f>'[1]Imperial Units'!I44*0.45359237</f>
+        <f>[1]Sheet1!I44*0.45359237</f>
         <v>0</v>
       </c>
       <c r="J44" s="4">
-        <f>'[1]Imperial Units'!J44</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <f>[1]Sheet1!J44</f>
+        <v>0</v>
+      </c>
+      <c r="S44" s="4"/>
+      <c r="U44" s="4"/>
+    </row>
+    <row r="45" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>2</v>
       </c>
       <c r="B45" s="3">
-        <f>'[1]Imperial Units'!B45</f>
+        <f>[1]Sheet1!B45</f>
         <v>0</v>
       </c>
       <c r="C45" s="3">
-        <f t="shared" ref="C45:C49" si="1">B45-$B$28</f>
+        <f t="shared" ref="C45:C49" si="2">B45-$B$28</f>
         <v>-0.65208333333333335</v>
       </c>
       <c r="D45" s="4">
-        <f>'[1]Imperial Units'!D45*0.3048</f>
+        <f>[1]Sheet1!D45*0.3048</f>
         <v>0</v>
       </c>
       <c r="E45" s="4">
-        <f>'[1]Imperial Units'!E45/0.514444</f>
+        <f>[1]Sheet1!E45/0.514444</f>
         <v>0</v>
       </c>
       <c r="F45" s="4">
-        <f>'[1]Imperial Units'!F45</f>
+        <f>[1]Sheet1!F45</f>
         <v>0</v>
       </c>
       <c r="G45" s="4">
-        <f>'[1]Imperial Units'!G45*0.45359237</f>
+        <f>[1]Sheet1!G45*0.45359237</f>
         <v>0</v>
       </c>
       <c r="H45" s="4">
-        <f>'[1]Imperial Units'!H45*0.45359237</f>
+        <f>[1]Sheet1!H45*0.45359237</f>
         <v>0</v>
       </c>
       <c r="I45" s="4">
-        <f>'[1]Imperial Units'!I45*0.45359237</f>
+        <f>[1]Sheet1!I45*0.45359237</f>
         <v>0</v>
       </c>
       <c r="J45" s="4">
-        <f>'[1]Imperial Units'!J45</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <f>[1]Sheet1!J45</f>
+        <v>0</v>
+      </c>
+      <c r="S45" s="4"/>
+      <c r="U45" s="4"/>
+    </row>
+    <row r="46" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>3</v>
       </c>
       <c r="B46" s="3">
-        <f>'[1]Imperial Units'!B46</f>
+        <f>[1]Sheet1!B46</f>
         <v>0</v>
       </c>
       <c r="C46" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.65208333333333335</v>
       </c>
       <c r="D46" s="4">
-        <f>'[1]Imperial Units'!D46*0.3048</f>
+        <f>[1]Sheet1!D46*0.3048</f>
         <v>0</v>
       </c>
       <c r="E46" s="4">
-        <f>'[1]Imperial Units'!E46/0.514444</f>
+        <f>[1]Sheet1!E46/0.514444</f>
         <v>0</v>
       </c>
       <c r="F46" s="4">
-        <f>'[1]Imperial Units'!F46</f>
+        <f>[1]Sheet1!F46</f>
         <v>0</v>
       </c>
       <c r="G46" s="4">
-        <f>'[1]Imperial Units'!G46*0.45359237</f>
+        <f>[1]Sheet1!G46*0.45359237</f>
         <v>0</v>
       </c>
       <c r="H46" s="4">
-        <f>'[1]Imperial Units'!H46*0.45359237</f>
+        <f>[1]Sheet1!H46*0.45359237</f>
         <v>0</v>
       </c>
       <c r="I46" s="4">
-        <f>'[1]Imperial Units'!I46*0.45359237</f>
+        <f>[1]Sheet1!I46*0.45359237</f>
         <v>0</v>
       </c>
       <c r="J46" s="4">
-        <f>'[1]Imperial Units'!J46</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <f>[1]Sheet1!J46</f>
+        <v>0</v>
+      </c>
+      <c r="S46" s="4"/>
+      <c r="U46" s="4"/>
+    </row>
+    <row r="47" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>4</v>
       </c>
       <c r="B47" s="3">
-        <f>'[1]Imperial Units'!B47</f>
+        <f>[1]Sheet1!B47</f>
         <v>0</v>
       </c>
       <c r="C47" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.65208333333333335</v>
       </c>
       <c r="D47" s="4">
-        <f>'[1]Imperial Units'!D47*0.3048</f>
+        <f>[1]Sheet1!D47*0.3048</f>
         <v>0</v>
       </c>
       <c r="E47" s="4">
-        <f>'[1]Imperial Units'!E47/0.514444</f>
+        <f>[1]Sheet1!E47/0.514444</f>
         <v>0</v>
       </c>
       <c r="F47" s="4">
-        <f>'[1]Imperial Units'!F47</f>
+        <f>[1]Sheet1!F47</f>
         <v>0</v>
       </c>
       <c r="G47" s="4">
-        <f>'[1]Imperial Units'!G47*0.45359237</f>
+        <f>[1]Sheet1!G47*0.45359237</f>
         <v>0</v>
       </c>
       <c r="H47" s="4">
-        <f>'[1]Imperial Units'!H47*0.45359237</f>
+        <f>[1]Sheet1!H47*0.45359237</f>
         <v>0</v>
       </c>
       <c r="I47" s="4">
-        <f>'[1]Imperial Units'!I47*0.45359237</f>
+        <f>[1]Sheet1!I47*0.45359237</f>
         <v>0</v>
       </c>
       <c r="J47" s="4">
-        <f>'[1]Imperial Units'!J47</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <f>[1]Sheet1!J47</f>
+        <v>0</v>
+      </c>
+      <c r="S47" s="4"/>
+      <c r="U47" s="4"/>
+    </row>
+    <row r="48" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>5</v>
       </c>
       <c r="B48" s="3">
-        <f>'[1]Imperial Units'!B48</f>
+        <f>[1]Sheet1!B48</f>
         <v>0</v>
       </c>
       <c r="C48" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.65208333333333335</v>
       </c>
       <c r="D48" s="4">
-        <f>'[1]Imperial Units'!D48*0.3048</f>
+        <f>[1]Sheet1!D48*0.3048</f>
         <v>0</v>
       </c>
       <c r="E48" s="4">
-        <f>'[1]Imperial Units'!E48/0.514444</f>
+        <f>[1]Sheet1!E48/0.514444</f>
         <v>0</v>
       </c>
       <c r="F48" s="4">
-        <f>'[1]Imperial Units'!F48</f>
+        <f>[1]Sheet1!F48</f>
         <v>0</v>
       </c>
       <c r="G48" s="4">
-        <f>'[1]Imperial Units'!G48*0.45359237</f>
+        <f>[1]Sheet1!G48*0.45359237</f>
         <v>0</v>
       </c>
       <c r="H48" s="4">
-        <f>'[1]Imperial Units'!H48*0.45359237</f>
+        <f>[1]Sheet1!H48*0.45359237</f>
         <v>0</v>
       </c>
       <c r="I48" s="4">
-        <f>'[1]Imperial Units'!I48*0.45359237</f>
+        <f>[1]Sheet1!I48*0.45359237</f>
         <v>0</v>
       </c>
       <c r="J48" s="4">
-        <f>'[1]Imperial Units'!J48</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <f>[1]Sheet1!J48</f>
+        <v>0</v>
+      </c>
+      <c r="S48" s="4"/>
+      <c r="U48" s="4"/>
+    </row>
+    <row r="49" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>6</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.65208333333333335</v>
       </c>
       <c r="D49" s="4">
-        <f>'[1]Imperial Units'!D49*0.3048</f>
+        <f>[1]Sheet1!D49*0.3048</f>
         <v>0</v>
       </c>
       <c r="E49" s="4">
-        <f>'[1]Imperial Units'!E49/0.514444</f>
+        <f>[1]Sheet1!E49/0.514444</f>
         <v>0</v>
       </c>
       <c r="F49" s="4">
-        <f>'[1]Imperial Units'!F49</f>
+        <f>[1]Sheet1!F49</f>
         <v>0</v>
       </c>
       <c r="G49" s="4">
-        <f>'[1]Imperial Units'!G49*0.45359237</f>
+        <f>[1]Sheet1!G49*0.45359237</f>
         <v>0</v>
       </c>
       <c r="H49" s="4">
-        <f>'[1]Imperial Units'!H49*0.45359237</f>
+        <f>[1]Sheet1!H49*0.45359237</f>
         <v>0</v>
       </c>
       <c r="I49" s="4">
-        <f>'[1]Imperial Units'!I49*0.45359237</f>
+        <f>[1]Sheet1!I49*0.45359237</f>
         <v>0</v>
       </c>
       <c r="J49" s="4">
-        <f>'[1]Imperial Units'!J49</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <f>[1]Sheet1!J49</f>
+        <v>0</v>
+      </c>
+      <c r="S49" s="4"/>
+      <c r="U49" s="4"/>
+    </row>
+    <row r="50" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>7</v>
       </c>
       <c r="B50" s="3"/>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="S50" s="4"/>
+      <c r="U50" s="4"/>
+    </row>
+    <row r="51" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="S51" s="4"/>
+      <c r="U51" s="4"/>
+    </row>
+    <row r="52" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="S52" s="4"/>
+      <c r="U52" s="4"/>
+    </row>
+    <row r="53" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="S53" s="4"/>
+      <c r="U53" s="4"/>
+    </row>
+    <row r="54" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>39</v>
       </c>
       <c r="D54" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="S54" s="4"/>
+      <c r="U54" s="4"/>
+    </row>
+    <row r="55" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="S55" s="4"/>
+      <c r="W55" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>18</v>
       </c>
@@ -2043,7 +2427,7 @@
       <c r="C56" t="s">
         <v>20</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E56" t="s">
@@ -2073,8 +2457,36 @@
       <c r="M56" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="S56" s="4"/>
+      <c r="T56" t="s">
+        <v>62</v>
+      </c>
+      <c r="W56" t="s">
+        <v>21</v>
+      </c>
+      <c r="X56" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y56" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z56" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA56" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC56" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD56" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE56" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="57" spans="1:31" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
         <v>28</v>
       </c>
@@ -2111,392 +2523,685 @@
       <c r="M57" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="S57" s="4"/>
+      <c r="T57" t="s">
+        <v>64</v>
+      </c>
+      <c r="W57" t="s">
+        <v>30</v>
+      </c>
+      <c r="X57" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y57" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z57" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA57" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC57" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD57" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE57" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="58" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="S58" s="4"/>
+      <c r="Y58" s="4"/>
+    </row>
+    <row r="59" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>1</v>
       </c>
       <c r="B59" s="5">
-        <f>'[1]Imperial Units'!B59</f>
+        <f>[1]Sheet1!B59</f>
         <v>2.013888888888889E-2</v>
       </c>
       <c r="C59" s="7">
-        <f>'[1]Imperial Units'!C59</f>
+        <f>[1]Sheet1!C59</f>
         <v>25</v>
       </c>
-      <c r="D59" s="7">
-        <f>'[1]Imperial Units'!D59*0.3048</f>
+      <c r="D59" s="12">
+        <f>[1]Sheet1!D59*0.3048</f>
         <v>1990.3440000000001</v>
       </c>
-      <c r="E59" s="7">
-        <f>'[1]Imperial Units'!E59/0.514444</f>
-        <v>311.01538748629588</v>
+      <c r="E59" s="11">
+        <f>[1]Sheet1!E59*0.514444</f>
+        <v>82.311040000000006</v>
       </c>
       <c r="F59" s="6">
-        <f>'[1]Imperial Units'!F59</f>
+        <f>[1]Sheet1!F59</f>
         <v>5.5</v>
       </c>
       <c r="G59" s="6">
-        <f>'[1]Imperial Units'!G59</f>
+        <f>[1]Sheet1!G59</f>
         <v>-0.1</v>
       </c>
       <c r="H59" s="6">
-        <f>'[1]Imperial Units'!H59</f>
+        <f>[1]Sheet1!H59</f>
         <v>3.1</v>
       </c>
       <c r="I59" s="7">
-        <f>'[1]Imperial Units'!I59</f>
+        <f>[1]Sheet1!I59</f>
         <v>-1</v>
       </c>
       <c r="J59" s="7">
-        <f>'[1]Imperial Units'!J59*0.45359237</f>
+        <f>[1]Sheet1!J59*0.45359237</f>
         <v>200.48782754000001</v>
       </c>
       <c r="K59" s="7">
-        <f>'[1]Imperial Units'!K59*0.45359237</f>
+        <f>[1]Sheet1!K59*0.45359237</f>
         <v>217.27074523000002</v>
       </c>
       <c r="L59" s="7">
-        <f>'[1]Imperial Units'!L59*0.45359237</f>
+        <f>[1]Sheet1!L59*0.45359237</f>
         <v>242.67191795000002</v>
       </c>
       <c r="M59" s="6">
-        <f>'[1]Imperial Units'!M59</f>
+        <f>[1]Sheet1!M59</f>
         <v>2.5</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="R59" s="4"/>
+      <c r="S59" s="4"/>
+      <c r="T59">
+        <f>(273.15+15) + 0.0065*D59</f>
+        <v>301.08723599999996</v>
+      </c>
+      <c r="W59" s="12">
+        <f>D59</f>
+        <v>1990.3440000000001</v>
+      </c>
+      <c r="X59" s="12">
+        <v>0.68086020544716597</v>
+      </c>
+      <c r="Y59" s="12">
+        <f>(273.15+M59)-T59</f>
+        <v>-25.437235999999984</v>
+      </c>
+      <c r="Z59" s="12">
+        <f>J59/3600</f>
+        <v>5.5691063205555558E-2</v>
+      </c>
+      <c r="AA59" s="12">
+        <f>K59/3600</f>
+        <v>6.0352984786111119E-2</v>
+      </c>
+      <c r="AC59">
+        <v>929.05399999999997</v>
+      </c>
+      <c r="AD59">
+        <v>1130.8499999999999</v>
+      </c>
+      <c r="AE59">
+        <f>AC59+AD59</f>
+        <v>2059.904</v>
+      </c>
+    </row>
+    <row r="60" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>2</v>
       </c>
       <c r="B60" s="5">
-        <f>'[1]Imperial Units'!B60</f>
+        <f>[1]Sheet1!B60</f>
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="C60" s="7">
-        <f>'[1]Imperial Units'!C60</f>
+        <f>[1]Sheet1!C60</f>
         <v>35</v>
       </c>
-      <c r="D60" s="7">
-        <f>'[1]Imperial Units'!D60*0.3048</f>
+      <c r="D60" s="12">
+        <f>[1]Sheet1!D60*0.3048</f>
         <v>2045.2080000000001</v>
       </c>
-      <c r="E60" s="7">
-        <f>'[1]Imperial Units'!E60/0.514444</f>
-        <v>289.63307959661302</v>
+      <c r="E60" s="11">
+        <f>[1]Sheet1!E60*0.514444</f>
+        <v>76.652156000000005</v>
       </c>
       <c r="F60" s="6">
-        <f>'[1]Imperial Units'!F60</f>
+        <f>[1]Sheet1!F60</f>
         <v>6.5</v>
       </c>
       <c r="G60" s="6">
-        <f>'[1]Imperial Units'!G60</f>
+        <f>[1]Sheet1!G60</f>
         <v>-0.4</v>
       </c>
       <c r="H60" s="6">
-        <f>'[1]Imperial Units'!H60</f>
+        <f>[1]Sheet1!H60</f>
         <v>3.1</v>
       </c>
       <c r="I60" s="7">
-        <f>'[1]Imperial Units'!I60</f>
+        <f>[1]Sheet1!I60</f>
         <v>-25</v>
       </c>
       <c r="J60" s="7">
-        <f>'[1]Imperial Units'!J60*0.45359237</f>
+        <f>[1]Sheet1!J60*0.45359237</f>
         <v>198.67345806</v>
       </c>
       <c r="K60" s="7">
-        <f>'[1]Imperial Units'!K60*0.45359237</f>
+        <f>[1]Sheet1!K60*0.45359237</f>
         <v>215.45637575000001</v>
       </c>
       <c r="L60" s="7">
-        <f>'[1]Imperial Units'!L60*0.45359237</f>
+        <f>[1]Sheet1!L60*0.45359237</f>
         <v>252.65095009000001</v>
       </c>
       <c r="M60" s="6">
-        <f>'[1]Imperial Units'!M60</f>
+        <f>[1]Sheet1!M60</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="R60" s="4"/>
+      <c r="S60" s="4"/>
+      <c r="T60">
+        <f>(273.15+15) + 0.0065*D60</f>
+        <v>301.44385199999999</v>
+      </c>
+      <c r="W60" s="12">
+        <f t="shared" ref="W60:W65" si="3">D60</f>
+        <v>2045.2080000000001</v>
+      </c>
+      <c r="X60" s="12">
+        <v>0.67602030437826199</v>
+      </c>
+      <c r="Y60" s="12">
+        <f>(273.15+M60)-T60</f>
+        <v>-26.293852000000015</v>
+      </c>
+      <c r="Z60" s="12">
+        <f>J60/3600</f>
+        <v>5.5187071683333332E-2</v>
+      </c>
+      <c r="AA60" s="12">
+        <f>K60/3600</f>
+        <v>5.9848993263888893E-2</v>
+      </c>
+      <c r="AC60">
+        <v>934.09699999999998</v>
+      </c>
+      <c r="AD60">
+        <v>1132.82</v>
+      </c>
+      <c r="AE60">
+        <f t="shared" ref="AE60:AE65" si="4">AC60+AD60</f>
+        <v>2066.9169999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>3</v>
       </c>
       <c r="B61" s="5">
-        <f>'[1]Imperial Units'!B61</f>
+        <f>[1]Sheet1!B61</f>
         <v>2.1527777777777781E-2</v>
       </c>
       <c r="C61" s="7">
-        <f>'[1]Imperial Units'!C61</f>
+        <f>[1]Sheet1!C61</f>
         <v>28</v>
       </c>
-      <c r="D61" s="7">
-        <f>'[1]Imperial Units'!D61*0.3048</f>
+      <c r="D61" s="12">
+        <f>[1]Sheet1!D61*0.3048</f>
         <v>2097.0239999999999</v>
       </c>
-      <c r="E61" s="7">
-        <f>'[1]Imperial Units'!E61/0.514444</f>
-        <v>272.1384640505089</v>
+      <c r="E61" s="11">
+        <f>[1]Sheet1!E61*0.514444</f>
+        <v>72.02216</v>
       </c>
       <c r="F61" s="6">
-        <f>'[1]Imperial Units'!F61</f>
+        <f>[1]Sheet1!F61</f>
         <v>7.5</v>
       </c>
       <c r="G61" s="6">
-        <f>'[1]Imperial Units'!G61</f>
+        <f>[1]Sheet1!G61</f>
         <v>-0.9</v>
       </c>
       <c r="H61" s="6">
-        <f>'[1]Imperial Units'!H61</f>
+        <f>[1]Sheet1!H61</f>
         <v>3.1</v>
       </c>
       <c r="I61" s="7">
-        <f>'[1]Imperial Units'!I61</f>
+        <f>[1]Sheet1!I61</f>
         <v>-39</v>
       </c>
       <c r="J61" s="7">
-        <f>'[1]Imperial Units'!J61*0.45359237</f>
+        <f>[1]Sheet1!J61*0.45359237</f>
         <v>196.85908858000002</v>
       </c>
       <c r="K61" s="7">
-        <f>'[1]Imperial Units'!K61*0.45359237</f>
+        <f>[1]Sheet1!K61*0.45359237</f>
         <v>213.64200627000002</v>
       </c>
       <c r="L61" s="7">
-        <f>'[1]Imperial Units'!L61*0.45359237</f>
+        <f>[1]Sheet1!L61*0.45359237</f>
         <v>257.64046616000002</v>
       </c>
       <c r="M61" s="6">
-        <f>'[1]Imperial Units'!M61</f>
+        <f>[1]Sheet1!M61</f>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="R61" s="4"/>
+      <c r="S61" s="4"/>
+      <c r="T61">
+        <f>(273.15+15) + 0.0065*D61</f>
+        <v>301.78065599999996</v>
+      </c>
+      <c r="W61" s="12">
+        <f t="shared" si="3"/>
+        <v>2097.0239999999999</v>
+      </c>
+      <c r="X61" s="12">
+        <v>0.67355662102931702</v>
+      </c>
+      <c r="Y61" s="12">
+        <f>(273.15+M61)-T61</f>
+        <v>-27.130655999999988</v>
+      </c>
+      <c r="Z61" s="12">
+        <f>J61/3600</f>
+        <v>5.4683080161111119E-2</v>
+      </c>
+      <c r="AA61" s="12">
+        <f>K61/3600</f>
+        <v>5.9345001741666674E-2</v>
+      </c>
+      <c r="AC61">
+        <v>932.93</v>
+      </c>
+      <c r="AD61">
+        <v>1132.54</v>
+      </c>
+      <c r="AE61">
+        <f t="shared" si="4"/>
+        <v>2065.4699999999998</v>
+      </c>
+    </row>
+    <row r="62" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>4</v>
       </c>
       <c r="B62" s="5">
-        <f>'[1]Imperial Units'!B62</f>
+        <f>[1]Sheet1!B62</f>
         <v>2.2916666666666669E-2</v>
       </c>
       <c r="C62" s="7">
-        <f>'[1]Imperial Units'!C62</f>
+        <f>[1]Sheet1!C62</f>
         <v>17</v>
       </c>
-      <c r="D62" s="7">
-        <f>'[1]Imperial Units'!D62*0.3048</f>
+      <c r="D62" s="12">
+        <f>[1]Sheet1!D62*0.3048</f>
         <v>2179.3200000000002</v>
       </c>
-      <c r="E62" s="7">
-        <f>'[1]Imperial Units'!E62/0.514444</f>
-        <v>252.70000233261541</v>
+      <c r="E62" s="11">
+        <f>[1]Sheet1!E62*0.514444</f>
+        <v>66.877719999999997</v>
       </c>
       <c r="F62" s="6">
-        <f>'[1]Imperial Units'!F62</f>
+        <f>[1]Sheet1!F62</f>
         <v>9.1</v>
       </c>
       <c r="G62" s="6">
-        <f>'[1]Imperial Units'!G62</f>
+        <f>[1]Sheet1!G62</f>
         <v>-1.5</v>
       </c>
       <c r="H62" s="6">
-        <f>'[1]Imperial Units'!H62</f>
+        <f>[1]Sheet1!H62</f>
         <v>3.1</v>
       </c>
       <c r="I62" s="7">
-        <f>'[1]Imperial Units'!I62</f>
+        <f>[1]Sheet1!I62</f>
         <v>-50</v>
       </c>
       <c r="J62" s="7">
-        <f>'[1]Imperial Units'!J62*0.45359237</f>
+        <f>[1]Sheet1!J62*0.45359237</f>
         <v>195.04471910000001</v>
       </c>
       <c r="K62" s="7">
-        <f>'[1]Imperial Units'!K62*0.45359237</f>
+        <f>[1]Sheet1!K62*0.45359237</f>
         <v>211.37404442000002</v>
       </c>
       <c r="L62" s="7">
-        <f>'[1]Imperial Units'!L62*0.45359237</f>
+        <f>[1]Sheet1!L62*0.45359237</f>
         <v>268.52668304000002</v>
       </c>
       <c r="M62" s="6">
-        <f>'[1]Imperial Units'!M62</f>
+        <f>[1]Sheet1!M62</f>
         <v>0.8</v>
       </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="R62" s="4"/>
+      <c r="S62" s="4"/>
+      <c r="T62">
+        <f>(273.15+15) + 0.0065*D62</f>
+        <v>302.31557999999995</v>
+      </c>
+      <c r="W62" s="12">
+        <f t="shared" si="3"/>
+        <v>2179.3200000000002</v>
+      </c>
+      <c r="X62" s="12">
+        <v>0.67469448764784301</v>
+      </c>
+      <c r="Y62" s="12">
+        <f>(273.15+M62)-T62</f>
+        <v>-28.365579999999966</v>
+      </c>
+      <c r="Z62" s="12">
+        <f>J62/3600</f>
+        <v>5.4179088638888893E-2</v>
+      </c>
+      <c r="AA62" s="12">
+        <f>K62/3600</f>
+        <v>5.8715012338888893E-2</v>
+      </c>
+      <c r="AC62">
+        <v>928.452</v>
+      </c>
+      <c r="AD62">
+        <v>1128.99</v>
+      </c>
+      <c r="AE62">
+        <f t="shared" si="4"/>
+        <v>2057.442</v>
+      </c>
+    </row>
+    <row r="63" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>5</v>
       </c>
       <c r="B63" s="5">
-        <f>'[1]Imperial Units'!B63</f>
+        <f>[1]Sheet1!B63</f>
         <v>2.361111111111111E-2</v>
       </c>
       <c r="C63" s="7">
-        <f>'[1]Imperial Units'!C63</f>
+        <f>[1]Sheet1!C63</f>
         <v>50</v>
       </c>
-      <c r="D63" s="7">
-        <f>'[1]Imperial Units'!D63*0.3048</f>
+      <c r="D63" s="12">
+        <f>[1]Sheet1!D63*0.3048</f>
         <v>1959.864</v>
       </c>
-      <c r="E63" s="7">
-        <f>'[1]Imperial Units'!E63/0.514444</f>
-        <v>332.39769537597874</v>
+      <c r="E63" s="11">
+        <f>[1]Sheet1!E63*0.514444</f>
+        <v>87.969924000000006</v>
       </c>
       <c r="F63" s="6">
-        <f>'[1]Imperial Units'!F63</f>
+        <f>[1]Sheet1!F63</f>
         <v>4.8</v>
       </c>
       <c r="G63" s="6">
-        <f>'[1]Imperial Units'!G63</f>
+        <f>[1]Sheet1!G63</f>
         <v>0.3</v>
       </c>
       <c r="H63" s="6">
-        <f>'[1]Imperial Units'!H63</f>
+        <f>[1]Sheet1!H63</f>
         <v>3.1</v>
       </c>
       <c r="I63" s="7">
-        <f>'[1]Imperial Units'!I63</f>
+        <f>[1]Sheet1!I63</f>
         <v>29</v>
       </c>
       <c r="J63" s="7">
-        <f>'[1]Imperial Units'!J63*0.45359237</f>
+        <f>[1]Sheet1!J63*0.45359237</f>
         <v>202.30219702000002</v>
       </c>
       <c r="K63" s="7">
-        <f>'[1]Imperial Units'!K63*0.45359237</f>
+        <f>[1]Sheet1!K63*0.45359237</f>
         <v>219.08511471</v>
       </c>
       <c r="L63" s="7">
-        <f>'[1]Imperial Units'!L63*0.45359237</f>
+        <f>[1]Sheet1!L63*0.45359237</f>
         <v>279.41289992000003</v>
       </c>
       <c r="M63" s="6">
-        <f>'[1]Imperial Units'!M63</f>
+        <f>[1]Sheet1!M63</f>
         <v>3.2</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="R63" s="4"/>
+      <c r="S63" s="4"/>
+      <c r="T63">
+        <f>(273.15+15) + 0.0065*D63</f>
+        <v>300.889116</v>
+      </c>
+      <c r="W63" s="12">
+        <f t="shared" si="3"/>
+        <v>1959.864</v>
+      </c>
+      <c r="X63" s="12">
+        <v>0.68961942393337505</v>
+      </c>
+      <c r="Y63" s="12">
+        <f>(273.15+M63)-T63</f>
+        <v>-24.539116000000035</v>
+      </c>
+      <c r="Z63" s="12">
+        <f>J63/3600</f>
+        <v>5.6195054727777784E-2</v>
+      </c>
+      <c r="AA63" s="12">
+        <f>K63/3600</f>
+        <v>6.0856976308333331E-2</v>
+      </c>
+      <c r="AC63">
+        <v>921.05499999999995</v>
+      </c>
+      <c r="AD63">
+        <v>1121.3</v>
+      </c>
+      <c r="AE63">
+        <f t="shared" si="4"/>
+        <v>2042.355</v>
+      </c>
+    </row>
+    <row r="64" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>6</v>
       </c>
       <c r="B64" s="5">
-        <f>'[1]Imperial Units'!B64</f>
+        <f>[1]Sheet1!B64</f>
         <v>2.4305555555555556E-2</v>
       </c>
       <c r="C64" s="7">
-        <f>'[1]Imperial Units'!C64</f>
+        <f>[1]Sheet1!C64</f>
         <v>36</v>
       </c>
-      <c r="D64" s="7">
-        <f>'[1]Imperial Units'!D64*0.3048</f>
+      <c r="D64" s="12">
+        <f>[1]Sheet1!D64*0.3048</f>
         <v>1813.5600000000002</v>
       </c>
-      <c r="E64" s="7">
-        <f>'[1]Imperial Units'!E64/0.514444</f>
-        <v>353.78000326566155</v>
+      <c r="E64" s="11">
+        <f>[1]Sheet1!E64*0.514444</f>
+        <v>93.628808000000006</v>
       </c>
       <c r="F64" s="6">
-        <f>'[1]Imperial Units'!F64</f>
+        <f>[1]Sheet1!F64</f>
         <v>4</v>
       </c>
       <c r="G64" s="6">
-        <f>'[1]Imperial Units'!G64</f>
+        <f>[1]Sheet1!G64</f>
         <v>0.6</v>
       </c>
       <c r="H64" s="6">
-        <f>'[1]Imperial Units'!H64</f>
+        <f>[1]Sheet1!H64</f>
         <v>3.1</v>
       </c>
       <c r="I64" s="7">
-        <f>'[1]Imperial Units'!I64</f>
+        <f>[1]Sheet1!I64</f>
         <v>43</v>
       </c>
       <c r="J64" s="7">
-        <f>'[1]Imperial Units'!J64*0.45359237</f>
+        <f>[1]Sheet1!J64*0.45359237</f>
         <v>206.38452835000001</v>
       </c>
       <c r="K64" s="7">
-        <f>'[1]Imperial Units'!K64*0.45359237</f>
+        <f>[1]Sheet1!K64*0.45359237</f>
         <v>222.71385367000002</v>
       </c>
       <c r="L64" s="7">
-        <f>'[1]Imperial Units'!L64*0.45359237</f>
+        <f>[1]Sheet1!L64*0.45359237</f>
         <v>288.03115495000003</v>
       </c>
       <c r="M64" s="6">
-        <f>'[1]Imperial Units'!M64</f>
+        <f>[1]Sheet1!M64</f>
         <v>4.2</v>
       </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="R64" s="4"/>
+      <c r="S64" s="4"/>
+      <c r="T64">
+        <f>(273.15+15) + 0.0065*D64</f>
+        <v>299.93813999999998</v>
+      </c>
+      <c r="W64" s="12">
+        <f t="shared" si="3"/>
+        <v>1813.5600000000002</v>
+      </c>
+      <c r="X64" s="12">
+        <v>0.68415393388841295</v>
+      </c>
+      <c r="Y64" s="12">
+        <f>(273.15+M64)-T64</f>
+        <v>-22.58814000000001</v>
+      </c>
+      <c r="Z64" s="12">
+        <f>J64/3600</f>
+        <v>5.7329035652777784E-2</v>
+      </c>
+      <c r="AA64" s="12">
+        <f>K64/3600</f>
+        <v>6.1864959352777783E-2</v>
+      </c>
+      <c r="AC64">
+        <v>936.947</v>
+      </c>
+      <c r="AD64">
+        <v>1137.07</v>
+      </c>
+      <c r="AE64">
+        <f t="shared" si="4"/>
+        <v>2074.0169999999998</v>
+      </c>
+    </row>
+    <row r="65" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>7</v>
       </c>
       <c r="B65" s="5">
-        <f>'[1]Imperial Units'!B65</f>
+        <f>[1]Sheet1!B65</f>
         <v>2.6388888888888889E-2</v>
       </c>
       <c r="C65" s="7">
-        <f>'[1]Imperial Units'!C65</f>
+        <f>[1]Sheet1!C65</f>
         <v>10</v>
       </c>
-      <c r="D65" s="7">
-        <f>'[1]Imperial Units'!D65*0.3048</f>
+      <c r="D65" s="12">
+        <f>[1]Sheet1!D65*0.3048</f>
         <v>1542.288</v>
       </c>
-      <c r="E65" s="7">
-        <f>'[1]Imperial Units'!E65/0.514444</f>
-        <v>369.33077263997637</v>
+      <c r="E65" s="11">
+        <f>[1]Sheet1!E65*0.514444</f>
+        <v>97.74436</v>
       </c>
       <c r="F65" s="6">
-        <f>'[1]Imperial Units'!F65</f>
+        <f>[1]Sheet1!F65</f>
         <v>3.6</v>
       </c>
       <c r="G65" s="6">
-        <f>'[1]Imperial Units'!G65</f>
+        <f>[1]Sheet1!G65</f>
         <v>0.9</v>
       </c>
       <c r="H65" s="6">
-        <f>'[1]Imperial Units'!H65</f>
+        <f>[1]Sheet1!H65</f>
         <v>3.1</v>
       </c>
       <c r="I65" s="7">
-        <f>'[1]Imperial Units'!I65</f>
+        <f>[1]Sheet1!I65</f>
         <v>79</v>
       </c>
       <c r="J65" s="7">
-        <f>'[1]Imperial Units'!J65*0.45359237</f>
+        <f>[1]Sheet1!J65*0.45359237</f>
         <v>211.37404442000002</v>
       </c>
       <c r="K65" s="7">
-        <f>'[1]Imperial Units'!K65*0.45359237</f>
+        <f>[1]Sheet1!K65*0.45359237</f>
         <v>228.61055448000002</v>
       </c>
       <c r="L65" s="7">
-        <f>'[1]Imperial Units'!L65*0.45359237</f>
+        <f>[1]Sheet1!L65*0.45359237</f>
         <v>303.90688790000002</v>
       </c>
       <c r="M65" s="6">
-        <f>'[1]Imperial Units'!M65</f>
+        <f>[1]Sheet1!M65</f>
         <v>6.8</v>
       </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="R65" s="4"/>
+      <c r="S65" s="4"/>
+      <c r="T65">
+        <f>(273.15+15) + 0.0065*D65</f>
+        <v>298.17487199999999</v>
+      </c>
+      <c r="W65" s="12">
+        <f t="shared" si="3"/>
+        <v>1542.288</v>
+      </c>
+      <c r="X65" s="12">
+        <v>0.65868768480291395</v>
+      </c>
+      <c r="Y65" s="12">
+        <f>(273.15+M65)-T65</f>
+        <v>-18.224872000000005</v>
+      </c>
+      <c r="Z65" s="12">
+        <f>J65/3600</f>
+        <v>5.8715012338888893E-2</v>
+      </c>
+      <c r="AA65" s="12">
+        <f>K65/3600</f>
+        <v>6.3502931800000009E-2</v>
+      </c>
+      <c r="AC65">
+        <v>974.15499999999997</v>
+      </c>
+      <c r="AD65">
+        <v>1178.0899999999999</v>
+      </c>
+      <c r="AE65">
+        <f t="shared" si="4"/>
+        <v>2152.2449999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="S66" s="4"/>
+      <c r="U66" s="4"/>
+    </row>
+    <row r="67" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="S67" s="4"/>
+      <c r="U67" s="4"/>
+    </row>
+    <row r="68" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="S68" s="4"/>
+      <c r="U68" s="4"/>
+    </row>
+    <row r="69" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="S69" s="4"/>
+      <c r="U69" s="4"/>
+    </row>
+    <row r="70" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>48</v>
       </c>
       <c r="C70" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="S70" s="4"/>
+      <c r="U70" s="4"/>
+    </row>
+    <row r="71" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>50</v>
       </c>
@@ -2509,8 +3214,16 @@
       <c r="G71" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="S71" s="4"/>
+      <c r="U71" s="4"/>
+    </row>
+    <row r="72" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="S72" s="4"/>
+      <c r="W72" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="73" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>18</v>
       </c>
@@ -2520,7 +3233,7 @@
       <c r="C73" t="s">
         <v>20</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D73" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E73" t="s">
@@ -2550,8 +3263,36 @@
       <c r="M73" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="S73" s="4"/>
+      <c r="T73" t="s">
+        <v>62</v>
+      </c>
+      <c r="W73" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="X73" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y73" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z73" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA73" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC73" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD73" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE73" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="74" spans="1:31" x14ac:dyDescent="0.35">
       <c r="B74" t="s">
         <v>28</v>
       </c>
@@ -2588,119 +3329,217 @@
       <c r="M74" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="S74" s="4"/>
+      <c r="T74" t="s">
+        <v>64</v>
+      </c>
+      <c r="W74" t="s">
+        <v>30</v>
+      </c>
+      <c r="X74" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y74" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z74" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA74" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC74" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD74" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE74" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="75" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>1</v>
       </c>
       <c r="B75" s="5">
-        <f>'[1]Imperial Units'!B75</f>
+        <f>[1]Sheet1!B75</f>
         <v>2.7083333333333334E-2</v>
       </c>
       <c r="C75" s="7">
-        <f>'[1]Imperial Units'!C75</f>
+        <f>[1]Sheet1!C75</f>
         <v>55</v>
       </c>
-      <c r="D75" s="7">
-        <f>'[1]Imperial Units'!D75*0.3048</f>
+      <c r="D75" s="11">
+        <f>[1]Sheet1!D75*0.3048</f>
         <v>1676.4</v>
       </c>
-      <c r="E75" s="7">
-        <f>'[1]Imperial Units'!E75/0.514444</f>
-        <v>309.07154131450653</v>
+      <c r="E75" s="11">
+        <f>[1]Sheet1!E75*0.514444</f>
+        <v>81.796596000000008</v>
       </c>
       <c r="F75" s="6">
-        <f>'[1]Imperial Units'!F75</f>
+        <f>[1]Sheet1!F75</f>
         <v>5.7</v>
       </c>
       <c r="G75" s="6">
-        <f>'[1]Imperial Units'!G75</f>
+        <f>[1]Sheet1!G75</f>
         <v>0</v>
       </c>
       <c r="H75" s="6">
-        <f>'[1]Imperial Units'!H75</f>
+        <f>[1]Sheet1!H75</f>
         <v>3.1</v>
       </c>
       <c r="I75" s="7">
-        <f>'[1]Imperial Units'!I75</f>
+        <f>[1]Sheet1!I75</f>
         <v>0</v>
       </c>
       <c r="J75" s="7">
-        <f>'[1]Imperial Units'!J75*0.45359237</f>
+        <f>[1]Sheet1!J75*0.45359237</f>
         <v>203.20938176000001</v>
       </c>
       <c r="K75" s="7">
-        <f>'[1]Imperial Units'!K75*0.45359237</f>
+        <f>[1]Sheet1!K75*0.45359237</f>
         <v>219.53870708000002</v>
       </c>
       <c r="L75" s="7">
-        <f>'[1]Imperial Units'!L75*0.45359237</f>
+        <f>[1]Sheet1!L75*0.45359237</f>
         <v>317.06106663000003</v>
       </c>
       <c r="M75" s="6">
-        <f>'[1]Imperial Units'!M75</f>
+        <f>[1]Sheet1!M75</f>
         <v>4.2</v>
       </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="R75" s="4"/>
+      <c r="S75" s="4"/>
+      <c r="T75">
+        <f>(273.15+15)+0.0065*D75</f>
+        <v>299.04659999999996</v>
+      </c>
+      <c r="W75" s="12">
+        <f>D75</f>
+        <v>1676.4</v>
+      </c>
+      <c r="X75" s="12">
+        <v>0.63758649772229303</v>
+      </c>
+      <c r="Y75" s="12">
+        <f>(273.15+M75)-T75</f>
+        <v>-21.696599999999989</v>
+      </c>
+      <c r="Z75" s="12">
+        <f>J75/3600</f>
+        <v>5.6447050488888893E-2</v>
+      </c>
+      <c r="AA75" s="12">
+        <f>K75/3600</f>
+        <v>6.0982974188888893E-2</v>
+      </c>
+      <c r="AC75">
+        <v>965.06899999999996</v>
+      </c>
+      <c r="AD75">
+        <v>1167.79</v>
+      </c>
+      <c r="AE75">
+        <f>AC75+AD75</f>
+        <v>2132.8589999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>2</v>
       </c>
       <c r="B76" s="5">
-        <f>'[1]Imperial Units'!B76</f>
+        <f>[1]Sheet1!B76</f>
         <v>2.8472222222222222E-2</v>
       </c>
       <c r="C76" s="7">
-        <f>'[1]Imperial Units'!C76</f>
+        <f>[1]Sheet1!C76</f>
         <v>37</v>
       </c>
-      <c r="D76" s="7">
-        <f>'[1]Imperial Units'!D76*0.3048</f>
+      <c r="D76" s="11">
+        <f>[1]Sheet1!D76*0.3048</f>
         <v>1697.7360000000001</v>
       </c>
-      <c r="E76" s="7">
-        <f>'[1]Imperial Units'!E76/0.514444</f>
-        <v>307.12769514271719</v>
+      <c r="E76" s="11">
+        <f>[1]Sheet1!E76*0.514444</f>
+        <v>81.282151999999996</v>
       </c>
       <c r="F76" s="6">
-        <f>'[1]Imperial Units'!F76</f>
+        <f>[1]Sheet1!F76</f>
         <v>5.9</v>
       </c>
       <c r="G76" s="6">
-        <f>'[1]Imperial Units'!G76</f>
+        <f>[1]Sheet1!G76</f>
         <v>-0.6</v>
       </c>
       <c r="H76" s="6">
-        <f>'[1]Imperial Units'!H76</f>
+        <f>[1]Sheet1!H76</f>
         <v>3.1</v>
       </c>
       <c r="I76" s="7">
-        <f>'[1]Imperial Units'!I76</f>
+        <f>[1]Sheet1!I76</f>
         <v>-33</v>
       </c>
       <c r="J76" s="7">
-        <f>'[1]Imperial Units'!J76*0.45359237</f>
+        <f>[1]Sheet1!J76*0.45359237</f>
         <v>202.75578939000002</v>
       </c>
       <c r="K76" s="7">
-        <f>'[1]Imperial Units'!K76*0.45359237</f>
+        <f>[1]Sheet1!K76*0.45359237</f>
         <v>219.08511471</v>
       </c>
       <c r="L76" s="7">
-        <f>'[1]Imperial Units'!L76*0.45359237</f>
+        <f>[1]Sheet1!L76*0.45359237</f>
         <v>329.30806061999999</v>
       </c>
       <c r="M76" s="6">
-        <f>'[1]Imperial Units'!M76</f>
+        <f>[1]Sheet1!M76</f>
         <v>4.2</v>
       </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="R76" s="4"/>
+      <c r="S76" s="4"/>
+      <c r="T76">
+        <f>(273.15+15)+0.0065*D76</f>
+        <v>299.18528399999997</v>
+      </c>
+      <c r="W76" s="12">
+        <f>D76</f>
+        <v>1697.7360000000001</v>
+      </c>
+      <c r="X76" s="12">
+        <v>0.63935923113652204</v>
+      </c>
+      <c r="Y76" s="12">
+        <f>(273.15+M76)-T76</f>
+        <v>-21.835284000000001</v>
+      </c>
+      <c r="Z76" s="12">
+        <f>J76/3600</f>
+        <v>5.6321052608333338E-2</v>
+      </c>
+      <c r="AA76" s="12">
+        <f>K76/3600</f>
+        <v>6.0856976308333331E-2</v>
+      </c>
+      <c r="AC76">
+        <v>962.26400000000001</v>
+      </c>
+      <c r="AD76">
+        <v>1164.95</v>
+      </c>
+      <c r="AE76">
+        <f>AC76+AD76</f>
+        <v>2127.2139999999999</v>
+      </c>
+    </row>
+    <row r="79" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D81" t="s">
         <v>57</v>
       </c>
@@ -2711,7 +3550,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D82" t="s">
         <v>28</v>
       </c>
@@ -2722,61 +3561,62 @@
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>55</v>
       </c>
       <c r="D83" s="3">
-        <f>'[1]Imperial Units'!D83</f>
+        <f>[1]Sheet1!D83</f>
         <v>2.9166666666666664E-2</v>
       </c>
       <c r="E83" s="3" t="str">
-        <f>'[1]Imperial Units'!E83</f>
+        <f>[1]Sheet1!E83</f>
         <v>Dutch Roll</v>
       </c>
       <c r="F83" s="3"/>
       <c r="G83" s="3">
-        <f>'[1]Imperial Units'!G83</f>
+        <f>[1]Sheet1!G83</f>
         <v>3.1944444444444449E-2</v>
       </c>
       <c r="H83" s="3" t="str">
-        <f>'[1]Imperial Units'!H83</f>
+        <f>[1]Sheet1!H83</f>
         <v>Aper. Roll</v>
       </c>
       <c r="I83" s="3"/>
       <c r="J83" s="3">
-        <f>'[1]Imperial Units'!J83</f>
+        <f>[1]Sheet1!J83</f>
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>56</v>
       </c>
       <c r="D84" s="3">
-        <f>'[1]Imperial Units'!D84</f>
+        <f>[1]Sheet1!D84</f>
         <v>3.125E-2</v>
       </c>
       <c r="E84" s="3" t="str">
-        <f>'[1]Imperial Units'!E84</f>
+        <f>[1]Sheet1!E84</f>
         <v>Dutch Roll YD</v>
       </c>
       <c r="F84" s="3"/>
       <c r="G84" s="3">
-        <f>'[1]Imperial Units'!G84</f>
+        <f>[1]Sheet1!G84</f>
         <v>3.2638888888888891E-2</v>
       </c>
       <c r="H84" s="3" t="str">
-        <f>'[1]Imperial Units'!H84</f>
+        <f>[1]Sheet1!H84</f>
         <v xml:space="preserve">Spiral </v>
       </c>
       <c r="I84" s="3"/>
       <c r="J84" s="3">
-        <f>'[1]Imperial Units'!J84</f>
+        <f>[1]Sheet1!J84</f>
         <v>3.6111111111111115E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Document not needed anymore I think
</commit_message>
<xml_diff>
--- a/Testflightdata/20200305_V3_metric.xlsx
+++ b/Testflightdata/20200305_V3_metric.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitch\Documents\TU Delft\BSc-3\AE3212-II Simulation, Verification &amp; Validation\Aerodynamics\31\B31\Testflightdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9CE49C-422C-4B40-AFF9-19CAFA55059E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F665EC06-0D80-4095-9DB7-6B7BC46A743B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{D344435E-CCBC-4168-9073-2AFFB31A2551}"/>
+    <workbookView xWindow="38290" yWindow="-5600" windowWidth="38620" windowHeight="21360" xr2:uid="{D344435E-CCBC-4168-9073-2AFFB31A2551}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>